<commit_message>
Completed Facial Recognition workflow
</commit_message>
<xml_diff>
--- a/Project2Final/FacialRecognitionSystem/facialRecConfig.xlsx
+++ b/Project2Final/FacialRecognitionSystem/facialRecConfig.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jagib\Documents\Revature\JewlzAndTheBoyz-EmailCategorizationBot-P2\Project2Final\FacialRecognitionSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50DF05A1-C06C-4E9B-AF5C-64E6D928B9FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168F4851-969A-433B-8C60-FBBB71C5C2FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3090" yWindow="-12795" windowWidth="21600" windowHeight="11325"/>
+    <workbookView xWindow="864" yWindow="768" windowWidth="21600" windowHeight="11328" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="config" sheetId="1" r:id="rId1"/>
+    <sheet name="DESKTOP-QTRODSM" sheetId="3" r:id="rId1"/>
+    <sheet name=" LAPTOP-I4SK7GBT" sheetId="4" r:id="rId2"/>
+    <sheet name="JGPC" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>PythonPath</t>
   </si>
@@ -33,11 +35,32 @@
   <si>
     <t>C:\Users\jagib\OneDrive\Desktop\IdentificationModule\</t>
   </si>
+  <si>
+    <t>relativePath</t>
+  </si>
+  <si>
+    <t>~/OneDrive/Desktop/IdentificationModule</t>
+  </si>
+  <si>
+    <t>C:/Users/patri/Desktop/IdentificationModule</t>
+  </si>
+  <si>
+    <t>C:\Users\patri\AppData\Local\Programs\Python\Python36</t>
+  </si>
+  <si>
+    <t>~/Desktop/IdentificationModule</t>
+  </si>
+  <si>
+    <t>C:\Users\Ohhey\AppData\Local\Programs\Python\Python36</t>
+  </si>
+  <si>
+    <t>C:\Users\Ohhey\Desktop\IdentificationModule</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -871,21 +894,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2615C5-26F7-42CC-87AF-0CFDCA738B0A}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -893,7 +919,100 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C617A2CD-8E17-453D-AC75-32E406F6F77E}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64A729B9-8B3A-45CA-9855-B5FA30160AA2}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>